<commit_message>
line graph, bar graph, themeContext color
</commit_message>
<xml_diff>
--- a/backend/temp_debug_report.xlsx
+++ b/backend/temp_debug_report.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,107 +467,87 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-01 01:54:32 PST</t>
+          <t>2025-05-02 10:01:27 PST</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Total URLs Scanned</t>
+          <t>Severity - Safe</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>360</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Total Threats Detected (High/Critical)</t>
+          <t>Severity - Low</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>117</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Severity - Safe</t>
+          <t>Severity - Medium</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Severity - Low</t>
+          <t>Severity - High</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>43</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Severity - Medium</t>
+          <t>Severity - Critical</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Severity - High</t>
+          <t>Source - User Scans</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>105</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Severity - Critical</t>
+          <t>Source - SMS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Source - Manual Scans</t>
+          <t>Source - Email</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Source - SMS Scans</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Source - Email Scans</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -582,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,77 +578,129 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Scans</t>
+          <t>Total Scans</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Phishing Scans</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Safe Scans</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>3</v>
       </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -726,12 +758,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-04-30T15:11:07.525000</t>
+          <t>2025-05-01T14:57:30.415000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://faaarkkbook.com</t>
+          <t>https://stingenergydrink.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -750,18 +782,18 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>11.2</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-04-30T12:43:31.420000</t>
+          <t>2025-05-01T14:40:53.492000</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://jorogoaol.com</t>
+          <t>https://stanozolol.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -780,18 +812,18 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>11.2</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-04-29T16:12:00.237000</t>
+          <t>2025-05-01T14:30:36.054000</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://jorgol.comm</t>
+          <t>https://oxandrolone.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -816,12 +848,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-04-29T13:57:24.363000</t>
+          <t>2025-05-01T14:30:10.386000</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://goooooogle.com</t>
+          <t>https://oxandrolone.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -840,18 +872,18 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>11.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-04-29T08:43:00.350000</t>
+          <t>2025-05-01T14:21:47.464000</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://utoob.com</t>
+          <t>https://oxymetholone.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -861,27 +893,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>97.3</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-04-29T03:57:13.465000</t>
+          <t>2025-05-01T14:21:25.546000</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.youtube.com</t>
+          <t>https://oxymetholone.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -900,18 +932,18 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-04-26T04:23:25.830000</t>
+          <t>2025-05-01T14:19:02.389000</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://trt.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -930,18 +962,18 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>11.9</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-04-26T04:14:37.529000</t>
+          <t>2025-05-01T13:48:16.342000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://tren.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -951,27 +983,27 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>11.9</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-04-26T04:11:31.899000</t>
+          <t>2025-05-01T13:47:34.016000</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://testone.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -981,27 +1013,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>11.9</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-04-26T03:22:42.027000</t>
+          <t>2025-05-01T11:14:05.148000</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://adawdasdaw.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1011,27 +1043,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>96.09999999999999</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-04-26T03:20:15.590000</t>
+          <t>2025-05-01T11:08:52.736000</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://adawdasdaw.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1041,32 +1073,32 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>96.09999999999999</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-04-26T03:17:48.908000</t>
+          <t>2025-05-01T06:29:01.604000</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>CONGRATS! Nanalo ka ng ₱50,000 mula sa GCash! I-claim sa: http://gcash-reward-claim.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1080,18 +1112,18 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>96.09999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-04-26T03:16:49.344000</t>
+          <t>2025-05-01T02:45:28.711000</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://provasencceja2025.site/</t>
+          <t>https://jorgggol.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1110,18 +1142,18 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>10.6</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-04-26T03:16:13.574000</t>
+          <t>2025-05-01T02:43:36.425000</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.google.com</t>
+          <t>https://agooogle.com</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1131,32 +1163,32 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-04-25T15:56:12.850000</t>
+          <t>2025-05-01T02:40:29.882000</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>knetww.com/LiveAPP</t>
+          <t>https://agooogle.com</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1170,18 +1202,18 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.9</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-04-25T15:49:41.113000</t>
+          <t>2025-04-30T20:20:33.928000</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://shopee.ph</t>
+          <t>https://mmaaaericu.com</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1200,529 +1232,529 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>2025-04-30T15:11:07.525000</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://faaarkkbook.com</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-04-30T12:43:31.420000</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://jorogoaol.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-04-29T16:12:00.237000</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://jorgol.comm</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-04-29T13:57:24.363000</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://goooooogle.com</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-04-29T08:43:00.350000</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://utoob.com</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-04-29T03:57:13.465000</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-04-26T04:23:25.830000</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://wwww.facbook.com</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-04-26T04:14:37.529000</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://wwww.facbook.com</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-04-26T04:11:31.899000</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://wwww.facbook.com</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-04-26T03:22:42.027000</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://atendimentocorretora.online</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-04-26T03:20:15.590000</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://atendimentocorretora.online</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-04-26T03:17:48.908000</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://atendimentocorretora.online</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-04-26T03:16:49.344000</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://provasencceja2025.site/</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-04-26T03:16:13.574000</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-04-25T15:56:12.850000</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>knetww.com/LiveAPP</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-04-25T15:49:41.113000</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://shopee.ph</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>2025-04-25T13:01:01.420000</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>Sugal hindi na need pumunta CAS1NO, pIay online at manalo araw araw, upto 8888 na welcome bonus, 24 hours cash in/out.
 Web: win-m.life</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>SMS</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>Phishing Detected</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="F34" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-04-25T12:45:13.360000</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2025-04-25T10:57:24.024000</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2025-04-25T08:56:27.561000</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2025-04-25T08:45:07.934000</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>https://tera.vin/BDOOnline</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2025-04-25T08:12:03.631000</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>https://phlpostso-gov.com/ph</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-04-25T08:07:23.586000</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-04-25T07:07:47.577000</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:45:25.861000</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://lmportal.uc.edu.ph</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:45:24.419000</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>https://lmportal.uc.edu.ph</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:42:20.723000</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>https://lmportal.uc.edu.ph</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:39:58.283000</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:39:55.002000</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:33:21.311000</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:33:17.589000</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:30:11.208000</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2025-04-24T22:30:10.807000</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>https://www.guayaquil.gob.ec</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>6.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-04-24T22:18:47.012000</t>
+          <t>2025-04-25T12:45:13.360000</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.youtube.com</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1741,18 +1773,18 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>6.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-04-24T22:18:45.246000</t>
+          <t>2025-04-25T10:57:24.024000</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.facebook.com</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1771,18 +1803,18 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>6.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-04-24T22:13:43.584000</t>
+          <t>2025-04-25T08:56:27.561000</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.youtube.com</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1801,18 +1833,18 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>6.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-04-24T22:13:40.278000</t>
+          <t>2025-04-25T08:45:07.934000</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://tera.vin/BDOOnline</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1831,18 +1863,18 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>6.1</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-04-24T22:05:21.607000</t>
+          <t>2025-04-25T08:12:03.631000</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://phlpostso-gov.com/ph</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1861,18 +1893,18 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>6.1</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-04-24T22:05:21.576000</t>
+          <t>2025-04-25T08:07:23.586000</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.instagram.com</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1891,18 +1923,18 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>6.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-04-24T21:43:20.981000</t>
+          <t>2025-04-25T07:07:47.577000</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.facebook.com</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1921,18 +1953,18 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>6.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-04-24T21:40:53.022000</t>
+          <t>2025-04-24T22:45:25.861000</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1951,18 +1983,18 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-04-24T21:38:53.424000</t>
+          <t>2025-04-24T22:45:24.419000</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1981,18 +2013,18 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-04-24T21:36:32.311000</t>
+          <t>2025-04-24T22:42:20.723000</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://teretzurwaalet.webflow.io</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2011,18 +2043,18 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>2.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-04-24T21:32:44.583000</t>
+          <t>2025-04-24T22:39:58.283000</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://teretzurwaalet.webflow.io</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2041,18 +2073,18 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>2.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-04-24T19:14:22.109000</t>
+          <t>2025-04-24T22:39:55.002000</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://ashleymadisonid.com/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2062,27 +2094,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>96.09999999999999</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:42.977000</t>
+          <t>2025-04-24T22:33:21.311000</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://grohwtsuppllemments.site/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2101,18 +2133,18 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:14.196000</t>
+          <t>2025-04-24T22:33:17.589000</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2122,27 +2154,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>95.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:14.104000</t>
+          <t>2025-04-24T22:30:11.208000</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2152,27 +2184,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>95.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:13.811000</t>
+          <t>2025-04-24T22:30:10.807000</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2182,27 +2214,27 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>95.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-04-24T19:12:38.635000</t>
+          <t>2025-04-24T22:18:47.012000</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://siat.info/D3WYKsWn</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2221,18 +2253,18 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>16.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-04-24T19:12:08.528000</t>
+          <t>2025-04-24T22:18:45.246000</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2242,27 +2274,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>96.09999999999999</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-04-24T19:11:52.477000</t>
+          <t>2025-04-24T22:13:43.584000</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://central-atendimentoseguro.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2281,18 +2313,18 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-04-24T19:11:20.495000</t>
+          <t>2025-04-24T22:13:40.278000</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://gsnews24.com/inst/index.html</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2302,27 +2334,27 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>96.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:57.016000</t>
+          <t>2025-04-24T22:05:21.607000</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>http://www.personaliteeee.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2332,27 +2364,27 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>96.3</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:33.250000</t>
+          <t>2025-04-24T22:05:21.576000</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2371,18 +2403,18 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>9.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:20.564000</t>
+          <t>2025-04-24T21:43:20.981000</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://avisos-sat.com.mx/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2401,18 +2433,18 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:41.229000</t>
+          <t>2025-04-24T21:40:53.022000</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://avisos-sat.com.mx/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2431,18 +2463,18 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:25.549000</t>
+          <t>2025-04-24T21:38:53.424000</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://biadigitalatendimento.ru.com/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2461,18 +2493,18 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:07.708000</t>
+          <t>2025-04-24T21:36:32.311000</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://validarnetempresax.com/suporte</t>
+          <t>https://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2491,18 +2523,18 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>10.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-04-24T19:08:42.755000</t>
+          <t>2025-04-24T21:32:44.583000</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://app-usaflex-online.myshopify.com/</t>
+          <t>https://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2512,27 +2544,27 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>95.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-04-24T19:07:12.978000</t>
+          <t>2025-04-24T19:14:22.109000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.pro-bet7k.com/</t>
+          <t>https://ashleymadisonid.com/</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2542,27 +2574,27 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>9.5</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:55.551000</t>
+          <t>2025-04-24T19:13:42.977000</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://caixageraldepositoseguranca.com/</t>
+          <t>https://grohwtsuppllemments.site/</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2587,12 +2619,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:31.515000</t>
+          <t>2025-04-24T19:13:14.196000</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://httpss-wwwv-roblox.com</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2611,18 +2643,18 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>96.3</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:11.094000</t>
+          <t>2025-04-24T19:13:14.104000</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www-the-graph.xyz</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2632,27 +2664,27 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>9.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-04-24T19:05:51.952000</t>
+          <t>2025-04-24T19:13:13.811000</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://robinhood-z.com</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2662,27 +2694,27 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>8.9</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-04-24T19:05:08.333000</t>
+          <t>2025-04-24T19:12:38.635000</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://multipiier-pendle.com</t>
+          <t>https://siat.info/D3WYKsWn</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2692,27 +2724,27 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>96.3</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-04-24T19:04:53.651000</t>
+          <t>2025-04-24T19:12:08.528000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://usualmoney.finance</t>
+          <t>https://atendimentocorretora.online</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2722,27 +2754,27 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>12.6</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-04-24T19:04:29.004000</t>
+          <t>2025-04-24T19:11:52.477000</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://dubai-token2049.cam</t>
+          <t>https://central-atendimentoseguro.com</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2752,27 +2784,27 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>97.09999999999999</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-04-24T19:03:55.231000</t>
+          <t>2025-04-24T19:11:20.495000</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>http://www.frosttreasuryconnects.com</t>
+          <t>https://gsnews24.com/inst/index.html</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2782,27 +2814,27 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>7.5</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-04-24T19:03:25.537000</t>
+          <t>2025-04-24T19:10:57.016000</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://enccejadescomplicado.site/</t>
+          <t>http://www.personaliteeee.com</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2821,18 +2853,18 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>96.09999999999999</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:53.490000</t>
+          <t>2025-04-24T19:10:33.250000</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://estudeemude.site/</t>
+          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2842,27 +2874,27 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>96.09999999999999</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:25.441000</t>
+          <t>2025-04-24T19:10:20.564000</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://provasencceja2025.site/</t>
+          <t>https://avisos-sat.com.mx/</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2872,27 +2904,27 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>96.90000000000001</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:00.323000</t>
+          <t>2025-04-24T19:09:41.229000</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://z568zimbra.weebly.com/</t>
+          <t>https://avisos-sat.com.mx/</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2911,18 +2943,18 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:46.782000</t>
+          <t>2025-04-24T19:09:25.549000</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://bankbac.weebly.com/</t>
+          <t>https://biadigitalatendimento.ru.com/</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2941,18 +2973,18 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:38.007000</t>
+          <t>2025-04-24T19:09:07.708000</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>http://secure-paypal-com-login.io</t>
+          <t>https://validarnetempresax.com/suporte</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2971,18 +3003,18 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>11.2</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:38.007000</t>
+          <t>2025-04-24T19:08:42.755000</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>http://secure-paypal-com-login.io</t>
+          <t>https://app-usaflex-online.myshopify.com/</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2992,27 +3024,27 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>11.2</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:08.338000</t>
+          <t>2025-04-24T19:07:12.978000</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>http://apple-support-login-error.ru</t>
+          <t>https://www.pro-bet7k.com/</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3031,18 +3063,18 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>11.2</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-04-24T19:00:53.705000</t>
+          <t>2025-04-24T19:06:55.551000</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>http://winner777.pro/sm</t>
+          <t>https://caixageraldepositoseguranca.com/</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3061,18 +3093,18 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>17.3</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-04-24T19:00:33.763000</t>
+          <t>2025-04-24T19:06:31.515000</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>http://teretzurwaalet.webflow.io</t>
+          <t>https://httpss-wwwv-roblox.com</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3082,32 +3114,32 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>10.6</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-04-24T18:34:45.232000</t>
+          <t>2025-04-24T19:06:11.094000</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Kumusta po?</t>
+          <t>https://www-the-graph.xyz</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3121,23 +3153,23 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>0.3</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-04-24T18:33:51.681000</t>
+          <t>2025-04-24T19:05:51.952000</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Pa may klase ako maya ka na tumawag</t>
+          <t>https://robinhood-z.com</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3151,578 +3183,578 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-04-24T18:32:50.262000</t>
+          <t>2025-04-24T19:05:08.333000</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hi, san ka na ba? </t>
+          <t>https://multipiier-pendle.com</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>0.6</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-04-24T18:32:31.473000</t>
+          <t>2025-04-24T19:04:53.651000</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hi, Kumusta araw mo? </t>
+          <t>https://usualmoney.finance</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0.7</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>2025-04-24T19:04:29.004000</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://dubai-token2049.cam</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>97.09999999999999</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:03:55.231000</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>http://www.frosttreasuryconnects.com</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:03:25.537000</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://enccejadescomplicado.site/</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:02:53.490000</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://estudeemude.site/</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:02:25.441000</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://provasencceja2025.site/</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>96.90000000000001</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:02:00.323000</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://z568zimbra.weebly.com/</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:01:46.782000</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://bankbac.weebly.com/</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:01:38.007000</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>http://secure-paypal-com-login.io</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:01:38.007000</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>http://secure-paypal-com-login.io</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:01:08.338000</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>http://apple-support-login-error.ru</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:00:53.705000</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>http://winner777.pro/sm</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-04-24T19:00:33.763000</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>http://teretzurwaalet.webflow.io</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>User Scan</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-04-24T18:34:45.232000</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Kumusta po?</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-04-24T18:33:51.681000</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Pa may klase ako maya ka na tumawag</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>SAFE</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-04-24T18:32:50.262000</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi, san ka na ba? </t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Safe Link Verified</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-04-24T18:32:31.473000</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi, Kumusta araw mo? </t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Phishing Detected</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
           <t>2025-04-24T18:31:09.977000</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B101" t="inlineStr">
         <is>
           <t>yLast 3 days, play online BARA-HA,you will have 30% change get XiaoMI/8999P.
 web: baraha-p.life</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>SMS</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E101" t="inlineStr">
         <is>
           <t>Phishing Detected</t>
         </is>
       </c>
-      <c r="F85" t="n">
+      <c r="F101" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>2025-04-24T18:24:41.336000</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>[Winner777] Free P300 daily login bonus, claim now. https://winner777.pro/sm</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F86" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>2025-04-24T18:13:51.875000</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>https://teretzurwaalet.webflow.io</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F87" t="n">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>2025-04-24T18:08:11.889000</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Ang Smart ay nagiimbita para kunin ang inyong 1,888 bonus. Ito ay matatanggap sa inyOng Acc0unt. URL: ww3467.pw/3tZBIuD</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F88" t="n">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>2025-04-24T18:00:46.080000</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Napaka ganda ng pasok ng Weekend! Dahil dito kay antiviruspedia.net/Live napaka daming B0nu$ naghihintay sayo, hindi lang yan dahil chance mo pang maging VIP!</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F89" t="n">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:50:52.032000</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>['http://wp8luck.com/']</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F90" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:35:38.939000</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>https://landing.twistysnetwork.com/?ats=eyJhIjoxMDc0NCwiYyI6NDQ3NDc0ODgsIm4iOjIsInMiOjYyLCJlIjo4OTQxLCJwIjo1N30=</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F91" t="n">
-        <v>97.90000000000001</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:26:46.463000</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>https://www.universityofcebu.net</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F92" t="n">
-        <v>95.8</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:26:22.534000</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>https://www.lmportal.uc.edu.ph</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F93" t="n">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:22:27.069000</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>https://gsnews24.com/inst/index.html</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Phishing Detected</t>
-        </is>
-      </c>
-      <c r="F94" t="n">
-        <v>96.5</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:21:31.024000</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>https://trezor.secure-hardware.io/</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F95" t="n">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:20:55.959000</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>https://sp-update.info/</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F96" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:20:08.418000</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F97" t="n">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:19:38.774000</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>https://zedny.com.sa/</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F98" t="n">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>2025-04-24T17:16:56.307000</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>https://xhhld.com/jcb/</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F99" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>2025-04-24T10:52:19.748000</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>https://tiktok.com</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F100" t="n">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>2025-04-24T09:17:35.321000</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>https://shopee.ph</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>User Scan</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>SAFE</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>Safe Link Verified</t>
-        </is>
-      </c>
-      <c r="F101" t="n">
-        <v>4.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "line graph, bar graph, themeContext color"
</commit_message>
<xml_diff>
--- a/backend/temp_debug_report.xlsx
+++ b/backend/temp_debug_report.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,87 +467,107 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-02 10:01:27 PST</t>
+          <t>2025-05-01 01:54:32 PST</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Severity - Safe</t>
+          <t>Total URLs Scanned</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>164</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Severity - Low</t>
+          <t>Total Threats Detected (High/Critical)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Severity - Medium</t>
+          <t>Severity - Safe</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Severity - High</t>
+          <t>Severity - Low</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>109</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Severity - Critical</t>
+          <t>Severity - Medium</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Source - User Scans</t>
+          <t>Severity - High</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Source - SMS</t>
+          <t>Severity - Critical</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Source - Email</t>
+          <t>Source - Manual Scans</t>
         </is>
       </c>
       <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Source - SMS Scans</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Source - Email Scans</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -562,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,129 +598,77 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total Scans</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Phishing Scans</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Safe Scans</t>
+          <t>Scans</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>3</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -758,12 +726,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-01T14:57:30.415000</t>
+          <t>2025-04-30T15:11:07.525000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://stingenergydrink.com</t>
+          <t>https://faaarkkbook.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -782,18 +750,18 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>10.6</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-01T14:40:53.492000</t>
+          <t>2025-04-30T12:43:31.420000</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://stanozolol.com</t>
+          <t>https://jorogoaol.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -812,18 +780,18 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>11.9</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-05-01T14:30:36.054000</t>
+          <t>2025-04-29T16:12:00.237000</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oxandrolone.com</t>
+          <t>https://jorgol.comm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -848,12 +816,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-05-01T14:30:10.386000</t>
+          <t>2025-04-29T13:57:24.363000</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oxandrolone.com</t>
+          <t>https://goooooogle.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -872,18 +840,18 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>10.6</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-01T14:21:47.464000</t>
+          <t>2025-04-29T08:43:00.350000</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oxymetholone.com</t>
+          <t>https://utoob.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -893,27 +861,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>10.6</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-05-01T14:21:25.546000</t>
+          <t>2025-04-29T03:57:13.465000</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oxymetholone.com</t>
+          <t>https://www.youtube.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -932,18 +900,18 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>10.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-05-01T14:19:02.389000</t>
+          <t>2025-04-26T04:23:25.830000</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://trt.com</t>
+          <t>https://wwww.facbook.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -962,18 +930,18 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>96.3</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-05-01T13:48:16.342000</t>
+          <t>2025-04-26T04:14:37.529000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://tren.com</t>
+          <t>https://wwww.facbook.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -983,27 +951,27 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>8.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-05-01T13:47:34.016000</t>
+          <t>2025-04-26T04:11:31.899000</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://testone.com</t>
+          <t>https://wwww.facbook.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1013,27 +981,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>11.2</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-05-01T11:14:05.148000</t>
+          <t>2025-04-26T03:22:42.027000</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://adawdasdaw.com</t>
+          <t>https://atendimentocorretora.online</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1043,27 +1011,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>11.2</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-05-01T11:08:52.736000</t>
+          <t>2025-04-26T03:20:15.590000</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://adawdasdaw.com</t>
+          <t>https://atendimentocorretora.online</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1073,32 +1041,32 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>11.2</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-05-01T06:29:01.604000</t>
+          <t>2025-04-26T03:17:48.908000</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CONGRATS! Nanalo ka ng ₱50,000 mula sa GCash! I-claim sa: http://gcash-reward-claim.com</t>
+          <t>https://atendimentocorretora.online</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1112,18 +1080,18 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-05-01T02:45:28.711000</t>
+          <t>2025-04-26T03:16:49.344000</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://jorgggol.com</t>
+          <t>https://provasencceja2025.site/</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1142,18 +1110,18 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>11.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-05-01T02:43:36.425000</t>
+          <t>2025-04-26T03:16:13.574000</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://agooogle.com</t>
+          <t>https://www.google.com</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1163,32 +1131,32 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>12.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-05-01T02:40:29.882000</t>
+          <t>2025-04-25T15:56:12.850000</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://agooogle.com</t>
+          <t>knetww.com/LiveAPP</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1202,18 +1170,18 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>12.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-04-30T20:20:33.928000</t>
+          <t>2025-04-25T15:49:41.113000</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://mmaaaericu.com</t>
+          <t>https://shopee.ph</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1232,48 +1200,49 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>11.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-04-30T15:11:07.525000</t>
+          <t>2025-04-25T13:01:01.420000</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://faaarkkbook.com</t>
+          <t>Sugal hindi na need pumunta CAS1NO, pIay online at manalo araw araw, upto 8888 na welcome bonus, 24 hours cash in/out.
+Web: win-m.life</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>11.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-04-30T12:43:31.420000</t>
+          <t>2025-04-25T12:45:13.360000</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://jorogoaol.com</t>
+          <t>https://www.youtube.com</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1292,18 +1261,18 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>11.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-04-29T16:12:00.237000</t>
+          <t>2025-04-25T10:57:24.024000</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://jorgol.comm</t>
+          <t>https://www.facebook.com</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1322,18 +1291,18 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>10.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-04-29T13:57:24.363000</t>
+          <t>2025-04-25T08:56:27.561000</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://goooooogle.com</t>
+          <t>https://www.youtube.com</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1352,18 +1321,18 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>11.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-04-29T08:43:00.350000</t>
+          <t>2025-04-25T08:45:07.934000</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://utoob.com</t>
+          <t>https://tera.vin/BDOOnline</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1373,27 +1342,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>97.3</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-04-29T03:57:13.465000</t>
+          <t>2025-04-25T08:12:03.631000</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.youtube.com</t>
+          <t>https://phlpostso-gov.com/ph</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1412,18 +1381,18 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-04-26T04:23:25.830000</t>
+          <t>2025-04-25T08:07:23.586000</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://www.instagram.com</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1433,27 +1402,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>11.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-04-26T04:14:37.529000</t>
+          <t>2025-04-25T07:07:47.577000</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://www.facebook.com</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1463,27 +1432,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>11.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-04-26T04:11:31.899000</t>
+          <t>2025-04-24T22:45:25.861000</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://wwww.facbook.com</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1493,27 +1462,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>11.9</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-04-26T03:22:42.027000</t>
+          <t>2025-04-24T22:45:24.419000</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1523,27 +1492,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>96.09999999999999</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-04-26T03:20:15.590000</t>
+          <t>2025-04-24T22:42:20.723000</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1553,27 +1522,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>96.09999999999999</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-04-26T03:17:48.908000</t>
+          <t>2025-04-24T22:39:58.283000</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1583,27 +1552,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>96.09999999999999</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-04-26T03:16:49.344000</t>
+          <t>2025-04-24T22:39:55.002000</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://provasencceja2025.site/</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1622,18 +1591,18 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>10.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-04-26T03:16:13.574000</t>
+          <t>2025-04-24T22:33:21.311000</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.google.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1652,48 +1621,48 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-04-25T15:56:12.850000</t>
+          <t>2025-04-24T22:33:17.589000</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>knetww.com/LiveAPP</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-04-25T15:49:41.113000</t>
+          <t>2025-04-24T22:30:11.208000</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://shopee.ph</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1712,49 +1681,48 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-04-25T13:01:01.420000</t>
+          <t>2025-04-24T22:30:10.807000</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sugal hindi na need pumunta CAS1NO, pIay online at manalo araw araw, upto 8888 na welcome bonus, 24 hours cash in/out.
-Web: win-m.life</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-04-25T12:45:13.360000</t>
+          <t>2025-04-24T22:18:47.012000</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1773,18 +1741,18 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-04-25T10:57:24.024000</t>
+          <t>2025-04-24T22:18:45.246000</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.facebook.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1803,18 +1771,18 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-04-25T08:56:27.561000</t>
+          <t>2025-04-24T22:13:43.584000</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.youtube.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1833,18 +1801,18 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-04-25T08:45:07.934000</t>
+          <t>2025-04-24T22:13:40.278000</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://tera.vin/BDOOnline</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1863,18 +1831,18 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>11.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-04-25T08:12:03.631000</t>
+          <t>2025-04-24T22:05:21.607000</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://phlpostso-gov.com/ph</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1893,18 +1861,18 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>11.2</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-04-25T08:07:23.586000</t>
+          <t>2025-04-24T22:05:21.576000</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.instagram.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1923,18 +1891,18 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-04-25T07:07:47.577000</t>
+          <t>2025-04-24T21:43:20.981000</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.facebook.com</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1953,18 +1921,18 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-04-24T22:45:25.861000</t>
+          <t>2025-04-24T21:40:53.022000</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://lmportal.uc.edu.ph</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1983,18 +1951,18 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-04-24T22:45:24.419000</t>
+          <t>2025-04-24T21:38:53.424000</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://lmportal.uc.edu.ph</t>
+          <t>https://www.guayaquil.gob.ec</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2013,18 +1981,18 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-04-24T22:42:20.723000</t>
+          <t>2025-04-24T21:36:32.311000</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://lmportal.uc.edu.ph</t>
+          <t>https://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2043,18 +2011,18 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>5.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-04-24T22:39:58.283000</t>
+          <t>2025-04-24T21:32:44.583000</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2073,18 +2041,18 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>6.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-04-24T22:39:55.002000</t>
+          <t>2025-04-24T19:14:22.109000</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://ashleymadisonid.com/</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2094,27 +2062,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>6.1</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-04-24T22:33:21.311000</t>
+          <t>2025-04-24T19:13:42.977000</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://grohwtsuppllemments.site/</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2133,18 +2101,18 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>6.1</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-04-24T22:33:17.589000</t>
+          <t>2025-04-24T19:13:14.196000</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2154,27 +2122,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>6.1</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-04-24T22:30:11.208000</t>
+          <t>2025-04-24T19:13:14.104000</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2184,27 +2152,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>6.1</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-04-24T22:30:10.807000</t>
+          <t>2025-04-24T19:13:13.811000</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://www.tusoatya.online/</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2214,27 +2182,27 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>6.1</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-04-24T22:18:47.012000</t>
+          <t>2025-04-24T19:12:38.635000</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://siat.info/D3WYKsWn</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2253,18 +2221,18 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>6.1</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-04-24T22:18:45.246000</t>
+          <t>2025-04-24T19:12:08.528000</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://atendimentocorretora.online</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2274,27 +2242,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>6.1</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-04-24T22:13:43.584000</t>
+          <t>2025-04-24T19:11:52.477000</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://central-atendimentoseguro.com</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2313,18 +2281,18 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>6.1</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-04-24T22:13:40.278000</t>
+          <t>2025-04-24T19:11:20.495000</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://gsnews24.com/inst/index.html</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2334,27 +2302,27 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>6.1</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-04-24T22:05:21.607000</t>
+          <t>2025-04-24T19:10:57.016000</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>http://www.personaliteeee.com</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2364,27 +2332,27 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>6.1</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-04-24T22:05:21.576000</t>
+          <t>2025-04-24T19:10:33.250000</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2403,18 +2371,18 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>6.1</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-04-24T21:43:20.981000</t>
+          <t>2025-04-24T19:10:20.564000</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://avisos-sat.com.mx/</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2433,18 +2401,18 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>6.1</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-04-24T21:40:53.022000</t>
+          <t>2025-04-24T19:09:41.229000</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://avisos-sat.com.mx/</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2463,18 +2431,18 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>6.1</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-04-24T21:38:53.424000</t>
+          <t>2025-04-24T19:09:25.549000</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.guayaquil.gob.ec</t>
+          <t>https://biadigitalatendimento.ru.com/</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2493,18 +2461,18 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>6.1</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-04-24T21:36:32.311000</t>
+          <t>2025-04-24T19:09:07.708000</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://teretzurwaalet.webflow.io</t>
+          <t>https://validarnetempresax.com/suporte</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2523,18 +2491,18 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>2.5</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-04-24T21:32:44.583000</t>
+          <t>2025-04-24T19:08:42.755000</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://teretzurwaalet.webflow.io</t>
+          <t>https://app-usaflex-online.myshopify.com/</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2544,27 +2512,27 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>2.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-04-24T19:14:22.109000</t>
+          <t>2025-04-24T19:07:12.978000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://ashleymadisonid.com/</t>
+          <t>https://www.pro-bet7k.com/</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2574,27 +2542,27 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>96.09999999999999</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:42.977000</t>
+          <t>2025-04-24T19:06:55.551000</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://grohwtsuppllemments.site/</t>
+          <t>https://caixageraldepositoseguranca.com/</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2619,12 +2587,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:14.196000</t>
+          <t>2025-04-24T19:06:31.515000</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://httpss-wwwv-roblox.com</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2643,18 +2611,18 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>95.5</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:14.104000</t>
+          <t>2025-04-24T19:06:11.094000</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://www-the-graph.xyz</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2664,27 +2632,27 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>95.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-04-24T19:13:13.811000</t>
+          <t>2025-04-24T19:05:51.952000</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.tusoatya.online/</t>
+          <t>https://robinhood-z.com</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2694,27 +2662,27 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>95.5</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-04-24T19:12:38.635000</t>
+          <t>2025-04-24T19:05:08.333000</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://siat.info/D3WYKsWn</t>
+          <t>https://multipiier-pendle.com</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2724,27 +2692,27 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>16.4</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-04-24T19:12:08.528000</t>
+          <t>2025-04-24T19:04:53.651000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://atendimentocorretora.online</t>
+          <t>https://usualmoney.finance</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2754,27 +2722,27 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>96.09999999999999</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-04-24T19:11:52.477000</t>
+          <t>2025-04-24T19:04:29.004000</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://central-atendimentoseguro.com</t>
+          <t>https://dubai-token2049.cam</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2784,27 +2752,27 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>10.6</v>
+        <v>97.09999999999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-04-24T19:11:20.495000</t>
+          <t>2025-04-24T19:03:55.231000</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://gsnews24.com/inst/index.html</t>
+          <t>http://www.frosttreasuryconnects.com</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2814,27 +2782,27 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>96.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:57.016000</t>
+          <t>2025-04-24T19:03:25.537000</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>http://www.personaliteeee.com</t>
+          <t>https://enccejadescomplicado.site/</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2853,18 +2821,18 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>96.3</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:33.250000</t>
+          <t>2025-04-24T19:02:53.490000</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
+          <t>https://estudeemude.site/</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2874,27 +2842,27 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>9.5</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-04-24T19:10:20.564000</t>
+          <t>2025-04-24T19:02:25.441000</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://avisos-sat.com.mx/</t>
+          <t>https://provasencceja2025.site/</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2904,27 +2872,27 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>10.6</v>
+        <v>96.90000000000001</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:41.229000</t>
+          <t>2025-04-24T19:02:00.323000</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://avisos-sat.com.mx/</t>
+          <t>https://z568zimbra.weebly.com/</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2943,18 +2911,18 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>10.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:25.549000</t>
+          <t>2025-04-24T19:01:46.782000</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://biadigitalatendimento.ru.com/</t>
+          <t>https://bankbac.weebly.com/</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2973,18 +2941,18 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>10.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-04-24T19:09:07.708000</t>
+          <t>2025-04-24T19:01:38.007000</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://validarnetempresax.com/suporte</t>
+          <t>http://secure-paypal-com-login.io</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3003,18 +2971,18 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>10.6</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-04-24T19:08:42.755000</t>
+          <t>2025-04-24T19:01:38.007000</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://app-usaflex-online.myshopify.com/</t>
+          <t>http://secure-paypal-com-login.io</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3024,27 +2992,27 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>95.5</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-04-24T19:07:12.978000</t>
+          <t>2025-04-24T19:01:08.338000</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.pro-bet7k.com/</t>
+          <t>http://apple-support-login-error.ru</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3063,18 +3031,18 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>9.5</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:55.551000</t>
+          <t>2025-04-24T19:00:53.705000</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://caixageraldepositoseguranca.com/</t>
+          <t>http://winner777.pro/sm</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3093,18 +3061,18 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>10.6</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:31.515000</t>
+          <t>2025-04-24T19:00:33.763000</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://httpss-wwwv-roblox.com</t>
+          <t>http://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3114,32 +3082,32 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>96.3</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-04-24T19:06:11.094000</t>
+          <t>2025-04-24T18:34:45.232000</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www-the-graph.xyz</t>
+          <t>Kumusta po?</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3153,23 +3121,23 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>9.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-04-24T19:05:51.952000</t>
+          <t>2025-04-24T18:33:51.681000</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://robinhood-z.com</t>
+          <t>Pa may klase ako maya ka na tumawag</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3183,83 +3151,84 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>8.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-04-24T19:05:08.333000</t>
+          <t>2025-04-24T18:32:50.262000</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://multipiier-pendle.com</t>
+          <t xml:space="preserve">Hi, san ka na ba? </t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>96.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-04-24T19:04:53.651000</t>
+          <t>2025-04-24T18:32:31.473000</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://usualmoney.finance</t>
+          <t xml:space="preserve">Hi, Kumusta araw mo? </t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>12.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-04-24T19:04:29.004000</t>
+          <t>2025-04-24T18:31:09.977000</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://dubai-token2049.cam</t>
+          <t>yLast 3 days, play online BARA-HA,you will have 30% change get XiaoMI/8999P.
+web: baraha-p.life</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3273,48 +3242,48 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>97.09999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-04-24T19:03:55.231000</t>
+          <t>2025-04-24T18:24:41.336000</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>http://www.frosttreasuryconnects.com</t>
+          <t>[Winner777] Free P300 daily login bonus, claim now. https://winner777.pro/sm</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>7.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-04-24T19:03:25.537000</t>
+          <t>2025-04-24T18:13:51.875000</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://enccejadescomplicado.site/</t>
+          <t>https://teretzurwaalet.webflow.io</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3324,32 +3293,32 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>96.09999999999999</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:53.490000</t>
+          <t>2025-04-24T18:08:11.889000</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://estudeemude.site/</t>
+          <t>Ang Smart ay nagiimbita para kunin ang inyong 1,888 bonus. Ito ay matatanggap sa inyOng Acc0unt. URL: ww3467.pw/3tZBIuD</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3363,23 +3332,23 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>96.09999999999999</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:25.441000</t>
+          <t>2025-04-24T18:00:46.080000</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://provasencceja2025.site/</t>
+          <t>Napaka ganda ng pasok ng Weekend! Dahil dito kay antiviruspedia.net/Live napaka daming B0nu$ naghihintay sayo, hindi lang yan dahil chance mo pang maging VIP!</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3393,48 +3362,48 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>96.90000000000001</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-04-24T19:02:00.323000</t>
+          <t>2025-04-24T17:50:52.032000</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://z568zimbra.weebly.com/</t>
+          <t>['http://wp8luck.com/']</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>User Scan</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:46.782000</t>
+          <t>2025-04-24T17:35:38.939000</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://bankbac.weebly.com/</t>
+          <t>https://landing.twistysnetwork.com/?ats=eyJhIjoxMDc0NCwiYyI6NDQ3NDc0ODgsIm4iOjIsInMiOjYyLCJlIjo4OTQxLCJwIjo1N30=</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3444,27 +3413,27 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>97.90000000000001</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:38.007000</t>
+          <t>2025-04-24T17:26:46.463000</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>http://secure-paypal-com-login.io</t>
+          <t>https://www.universityofcebu.net</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3474,27 +3443,27 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>11.2</v>
+        <v>95.8</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:38.007000</t>
+          <t>2025-04-24T17:26:22.534000</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>http://secure-paypal-com-login.io</t>
+          <t>https://www.lmportal.uc.edu.ph</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3513,18 +3482,18 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>11.2</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-04-24T19:01:08.338000</t>
+          <t>2025-04-24T17:22:27.069000</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>http://apple-support-login-error.ru</t>
+          <t>https://gsnews24.com/inst/index.html</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3534,27 +3503,27 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>SAFE</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Safe Link Verified</t>
+          <t>Phishing Detected</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>11.2</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-04-24T19:00:53.705000</t>
+          <t>2025-04-24T17:21:31.024000</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>http://winner777.pro/sm</t>
+          <t>https://trezor.secure-hardware.io/</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3573,18 +3542,18 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>17.3</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-04-24T19:00:33.763000</t>
+          <t>2025-04-24T17:20:55.959000</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>http://teretzurwaalet.webflow.io</t>
+          <t>https://sp-update.info/</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3603,23 +3572,23 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>10.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-04-24T18:34:45.232000</t>
+          <t>2025-04-24T17:20:08.418000</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Kumusta po?</t>
+          <t>https://sbi-accessconfirm.zfssw.com/page/</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3633,23 +3602,23 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>0.3</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-04-24T18:33:51.681000</t>
+          <t>2025-04-24T17:19:38.774000</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Pa may klase ako maya ka na tumawag</t>
+          <t>https://zedny.com.sa/</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3663,28 +3632,28 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-04-24T18:32:50.262000</t>
+          <t>2025-04-24T17:16:56.307000</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hi, san ka na ba? </t>
+          <t>https://xhhld.com/jcb/</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3693,68 +3662,67 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>0.6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-04-24T18:32:31.473000</t>
+          <t>2025-04-24T10:52:19.748000</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hi, Kumusta araw mo? </t>
+          <t>https://tiktok.com</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>0.7</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-04-24T18:31:09.977000</t>
+          <t>2025-04-24T09:17:35.321000</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>yLast 3 days, play online BARA-HA,you will have 30% change get XiaoMI/8999P.
-web: baraha-p.life</t>
+          <t>https://shopee.ph</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>User Scan</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>SAFE</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Phishing Detected</t>
+          <t>Safe Link Verified</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>4.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>